<commit_message>
200203 ball/item modified, ball probability change, Playerprefabs(User_stage) add
</commit_message>
<xml_diff>
--- a/할일정리파일.xlsx
+++ b/할일정리파일.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\Game_MoonRabbit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{269F7110-95E7-4F20-B394-B6E78651C62D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{080289D8-F855-4B3E-A481-0FDDB48C6C48}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{A399527B-BAE3-45DA-870A-D71D4B42C21D}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="48">
   <si>
     <t>프로그래밍</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -221,6 +221,20 @@
   </si>
   <si>
     <t>아이템 물음표 상자</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>O
+-10/+2.5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>O
+User_stage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>최준아</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -600,12 +614,13 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="29.75" customWidth="1"/>
+    <col min="2" max="2" width="10" customWidth="1"/>
     <col min="3" max="3" width="29.25" customWidth="1"/>
     <col min="5" max="5" width="34.125" customWidth="1"/>
   </cols>
@@ -625,8 +640,8 @@
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
-        <v>36</v>
+      <c r="B2" s="2" t="s">
+        <v>45</v>
       </c>
       <c r="C2" t="s">
         <v>21</v>
@@ -669,12 +684,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="33" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="B5" t="s">
-        <v>36</v>
+      <c r="B5" s="2" t="s">
+        <v>46</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>41</v>
@@ -729,7 +744,7 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C10" t="s">
         <v>26</v>
@@ -758,6 +773,9 @@
       <c r="A13" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="B13" t="s">
+        <v>47</v>
+      </c>
       <c r="C13" t="s">
         <v>30</v>
       </c>
@@ -819,7 +837,7 @@
         <v>37</v>
       </c>
       <c r="B19" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
200204 ball modified, ball probability modified
</commit_message>
<xml_diff>
--- a/할일정리파일.xlsx
+++ b/할일정리파일.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\Game_MoonRabbit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{080289D8-F855-4B3E-A481-0FDDB48C6C48}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0DB5809-5400-469F-964C-C61B284F1633}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{A399527B-BAE3-45DA-870A-D71D4B42C21D}"/>
+    <workbookView xWindow="1200" yWindow="240" windowWidth="11025" windowHeight="10320" xr2:uid="{A399527B-BAE3-45DA-870A-D71D4B42C21D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="49">
   <si>
     <t>프로그래밍</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -225,16 +225,20 @@
   </si>
   <si>
     <t>O
--10/+2.5</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>O
 User_stage</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>최준아</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rowbomb, sixbomb 제일 밑에서 
+쏘면 폭탄 소리 안나고 구슬 쌓이는 소리 남</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>O</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -611,10 +615,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AD2D038-EFC7-40D9-8F02-588A133B84E6}">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -641,7 +645,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s">
         <v>21</v>
@@ -684,12 +688,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="33" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>41</v>
@@ -774,7 +778,7 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C13" t="s">
         <v>30</v>
@@ -843,6 +847,14 @@
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
200204 ball probability modified
</commit_message>
<xml_diff>
--- a/할일정리파일.xlsx
+++ b/할일정리파일.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Game_MoonRabbit\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\Game_MoonRabbit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB6A7A28-5B2A-4962-9020-D6C5EF838CF5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DEAC5C0-06BF-4613-973A-66CCAEAE0043}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{A399527B-BAE3-45DA-870A-D71D4B42C21D}"/>
+    <workbookView xWindow="1200" yWindow="240" windowWidth="11025" windowHeight="10320" xr2:uid="{A399527B-BAE3-45DA-870A-D71D4B42C21D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -621,19 +621,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AD2D038-EFC7-40D9-8F02-588A133B84E6}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="29.75" customWidth="1"/>
     <col min="2" max="2" width="10" customWidth="1"/>
     <col min="3" max="3" width="29.25" customWidth="1"/>
-    <col min="5" max="5" width="34.08203125" customWidth="1"/>
+    <col min="5" max="5" width="34.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -644,12 +644,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="68" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" ht="66" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s">
         <v>21</v>
@@ -664,7 +664,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -678,7 +678,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -692,7 +692,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="34" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" ht="33" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -706,7 +706,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="51" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>40</v>
       </c>
@@ -717,7 +717,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="34" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" ht="33" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -728,7 +728,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="34" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" ht="33" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -739,7 +739,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="34" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" ht="33" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -747,7 +747,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -758,7 +758,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="51" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -766,7 +766,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="34" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" ht="33" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
@@ -777,7 +777,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>13</v>
       </c>
@@ -788,7 +788,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>14</v>
       </c>
@@ -799,7 +799,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>15</v>
       </c>
@@ -807,7 +807,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>16</v>
       </c>
@@ -818,7 +818,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>18</v>
       </c>
@@ -832,7 +832,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>17</v>
       </c>
@@ -840,7 +840,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="51" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:4" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>37</v>
       </c>
@@ -848,12 +848,12 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="51" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:4" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>47</v>
       </c>

</xml_diff>

<commit_message>
200210 art add, ui art add
</commit_message>
<xml_diff>
--- a/할일정리파일.xlsx
+++ b/할일정리파일.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\Game_MoonRabbit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8683B74B-709B-479B-AE3C-F13845990AAB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9B2898F-5E92-4C2E-88D7-49537C1406C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6420" yWindow="45" windowWidth="11025" windowHeight="10320" xr2:uid="{A399527B-BAE3-45DA-870A-D71D4B42C21D}"/>
+    <workbookView xWindow="7350" yWindow="270" windowWidth="11025" windowHeight="10320" xr2:uid="{A399527B-BAE3-45DA-870A-D71D4B42C21D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="57">
   <si>
     <t>프로그래밍</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -85,10 +85,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>UI 적용(퀘스트구슬 표시/ 일시중지 창-다시시작,뒤로가기/ 배경음,효과음켜고끄기)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>(+2, -2)구슬 먹을때 크기 줄었다커졌다</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -251,6 +247,31 @@
   </si>
   <si>
     <t>친구</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">stage option 창에서 restart 버튼 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>stage에서 퀘스트구슬 개수 표시</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wall_left, wall_right, whitewall_left,
+whitewall_right를 stage_Night2로 다시 적용.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5, 10. 15 stage에서 퀘스트완료하면 일러스트 뜨게, 20stage끝나면 클리어 일러스트 뜨게.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UI 이미지 적용(퀘스트구슬 표시/ 일시중지 창-다시시작,뒤로가기/ 배경음,효과음켜고끄기)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>O</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -627,10 +648,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AD2D038-EFC7-40D9-8F02-588A133B84E6}">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -657,19 +678,19 @@
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>39</v>
-      </c>
       <c r="F2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -677,16 +698,16 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -694,16 +715,16 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="33" x14ac:dyDescent="0.3">
@@ -711,24 +732,24 @@
         <v>6</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="33" x14ac:dyDescent="0.3">
@@ -736,10 +757,10 @@
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="33" x14ac:dyDescent="0.3">
@@ -747,10 +768,10 @@
         <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="33" x14ac:dyDescent="0.3">
@@ -758,10 +779,10 @@
         <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -769,116 +790,137 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>11</v>
+        <v>55</v>
+      </c>
+      <c r="B11" t="s">
+        <v>56</v>
       </c>
       <c r="C11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="33" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C16" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" t="s">
         <v>34</v>
-      </c>
-      <c r="D16" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D17" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="66" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>35</v>
+        <v>34</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" t="s">
         <v>37</v>
-      </c>
-      <c r="B19" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" t="s">
         <v>46</v>
       </c>
-      <c r="B21" t="s">
-        <v>47</v>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
200211 ball line ing
</commit_message>
<xml_diff>
--- a/할일정리파일.xlsx
+++ b/할일정리파일.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\Game_MoonRabbit\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Game_MoonRabbit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9B2898F-5E92-4C2E-88D7-49537C1406C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5754B78-E4D0-4DB9-9A1C-BB9070597EAF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7350" yWindow="270" windowWidth="11025" windowHeight="10320" xr2:uid="{A399527B-BAE3-45DA-870A-D71D4B42C21D}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{A399527B-BAE3-45DA-870A-D71D4B42C21D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="57">
   <si>
     <t>프로그래밍</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -650,19 +650,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AD2D038-EFC7-40D9-8F02-588A133B84E6}">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="29.75" customWidth="1"/>
     <col min="2" max="2" width="10" customWidth="1"/>
     <col min="3" max="3" width="29.25" customWidth="1"/>
-    <col min="5" max="5" width="34.125" customWidth="1"/>
+    <col min="5" max="5" width="34.08203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -673,7 +673,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="66" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="68" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -693,7 +693,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -710,7 +710,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -727,7 +727,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="33" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="34" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -741,7 +741,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="51" x14ac:dyDescent="0.45">
       <c r="A6" s="2" t="s">
         <v>39</v>
       </c>
@@ -752,7 +752,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="33" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="34" x14ac:dyDescent="0.45">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -763,7 +763,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="33" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="34" x14ac:dyDescent="0.45">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -774,7 +774,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="33" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="34" x14ac:dyDescent="0.45">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -785,7 +785,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -799,7 +799,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="51" x14ac:dyDescent="0.45">
       <c r="A11" s="2" t="s">
         <v>55</v>
       </c>
@@ -810,7 +810,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="33" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="34" x14ac:dyDescent="0.45">
       <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
@@ -821,7 +821,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
@@ -832,7 +832,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
@@ -843,7 +843,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
@@ -851,7 +851,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
@@ -862,7 +862,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17" s="2" t="s">
         <v>17</v>
       </c>
@@ -876,7 +876,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="66" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" ht="51" x14ac:dyDescent="0.45">
       <c r="A18" s="2" t="s">
         <v>16</v>
       </c>
@@ -886,8 +886,11 @@
       <c r="C18" s="2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="D18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="51" x14ac:dyDescent="0.45">
       <c r="A19" s="2" t="s">
         <v>36</v>
       </c>
@@ -895,12 +898,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A20" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" ht="51" x14ac:dyDescent="0.45">
       <c r="A21" s="2" t="s">
         <v>45</v>
       </c>
@@ -908,17 +911,17 @@
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A22" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A23" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" ht="51" x14ac:dyDescent="0.45">
       <c r="A24" s="2" t="s">
         <v>54</v>
       </c>

</xml_diff>

<commit_message>
200212 animations add, clear/fail modified
</commit_message>
<xml_diff>
--- a/할일정리파일.xlsx
+++ b/할일정리파일.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Game_MoonRabbit\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\Game_MoonRabbit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5754B78-E4D0-4DB9-9A1C-BB9070597EAF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9EAF18C-B75E-4DEA-9A73-7E6243D7BF55}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{A399527B-BAE3-45DA-870A-D71D4B42C21D}"/>
+    <workbookView xWindow="7350" yWindow="270" windowWidth="11025" windowHeight="10320" xr2:uid="{A399527B-BAE3-45DA-870A-D71D4B42C21D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="55">
   <si>
     <t>프로그래밍</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -181,10 +181,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>최준아</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>구슬 코딩 고치기 (rainbow 돌, 중앙에서도 터지게, ball바꾸기, rainbow 폭탄에 닿았을때 안멈춤)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -238,18 +234,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>최준아</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>친구</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>친구</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve">stage option 창에서 restart 버튼 </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -272,6 +256,15 @@
   </si>
   <si>
     <t>O</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>최준아</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>송여령
+(쿠키런B)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -650,19 +643,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AD2D038-EFC7-40D9-8F02-588A133B84E6}">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="29.75" customWidth="1"/>
     <col min="2" max="2" width="10" customWidth="1"/>
     <col min="3" max="3" width="29.25" customWidth="1"/>
-    <col min="5" max="5" width="34.08203125" customWidth="1"/>
+    <col min="5" max="5" width="34.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -673,27 +666,27 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="68" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" ht="66" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s">
         <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -704,113 +697,128 @@
         <v>21</v>
       </c>
       <c r="D3" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="E3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" ht="33" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
-        <v>34</v>
+      <c r="B4" s="2" t="s">
+        <v>54</v>
       </c>
       <c r="C4" t="s">
         <v>22</v>
       </c>
       <c r="D4" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="E4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="34" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" ht="33" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="51" x14ac:dyDescent="0.45">
-      <c r="A6" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>41</v>
-      </c>
       <c r="D6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="34" x14ac:dyDescent="0.45">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="33" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="B7" s="2" t="s">
+        <v>53</v>
+      </c>
       <c r="C7" t="s">
         <v>23</v>
       </c>
       <c r="D7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="34" x14ac:dyDescent="0.45">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="33" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="B8" t="s">
+        <v>53</v>
+      </c>
       <c r="C8" t="s">
         <v>24</v>
       </c>
       <c r="D8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="34" x14ac:dyDescent="0.45">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="33" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="B9" t="s">
+        <v>53</v>
+      </c>
       <c r="C9" t="s">
         <v>28</v>
       </c>
       <c r="D9" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C10" t="s">
         <v>25</v>
       </c>
       <c r="D10" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="51" x14ac:dyDescent="0.45">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B11" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C11" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="34" x14ac:dyDescent="0.45">
+      <c r="D11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="33" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
@@ -818,21 +826,21 @@
         <v>27</v>
       </c>
       <c r="D12" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C13" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
@@ -843,7 +851,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
@@ -851,7 +859,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
@@ -862,21 +870,21 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D17" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="51" x14ac:dyDescent="0.45">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="66" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>16</v>
       </c>
@@ -884,46 +892,46 @@
         <v>34</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D18" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="51" x14ac:dyDescent="0.45">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B19" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="51" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:4" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" t="s">
         <v>45</v>
       </c>
-      <c r="B21" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="51" x14ac:dyDescent="0.45">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
200212 animation add, map lock add, character lock add, prefab modified
</commit_message>
<xml_diff>
--- a/할일정리파일.xlsx
+++ b/할일정리파일.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\Game_MoonRabbit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9EAF18C-B75E-4DEA-9A73-7E6243D7BF55}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{058DD224-009D-4636-9A34-F0BE9915039C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7350" yWindow="270" windowWidth="11025" windowHeight="10320" xr2:uid="{A399527B-BAE3-45DA-870A-D71D4B42C21D}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="56">
   <si>
     <t>프로그래밍</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -265,6 +265,10 @@
   <si>
     <t>송여령
 (쿠키런B)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>O</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -643,8 +647,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AD2D038-EFC7-40D9-8F02-588A133B84E6}">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -739,7 +743,7 @@
         <v>38</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>40</v>
@@ -753,7 +757,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="C7" t="s">
         <v>23</v>
@@ -767,7 +771,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="C8" t="s">
         <v>24</v>
@@ -922,6 +926,9 @@
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>47</v>
+      </c>
+      <c r="B22" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
200212 rabbit jump animation modified
</commit_message>
<xml_diff>
--- a/할일정리파일.xlsx
+++ b/할일정리파일.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\Game_MoonRabbit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{058DD224-009D-4636-9A34-F0BE9915039C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B15ACCF-5B41-4151-9487-E7D454DC8AC5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7350" yWindow="270" windowWidth="11025" windowHeight="10320" xr2:uid="{A399527B-BAE3-45DA-870A-D71D4B42C21D}"/>
+    <workbookView xWindow="1440" yWindow="300" windowWidth="11025" windowHeight="10320" xr2:uid="{A399527B-BAE3-45DA-870A-D71D4B42C21D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="59">
   <si>
     <t>프로그래밍</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -269,6 +269,18 @@
   </si>
   <si>
     <t>O</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>item사용 결정에 따른 코딩</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>item눌러서 사용시 애니메이터 추가 필요(현재 sprite변경으로 이루어져서)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>구슬 애니메이션이 destroy되기전에 먼저 이루어지도록 해야함.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -645,10 +657,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AD2D038-EFC7-40D9-8F02-588A133B84E6}">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -941,6 +953,21 @@
         <v>50</v>
       </c>
     </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="33" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
200214 stageclear add, ball animation modified, items modified, ball position modified, Start position modified, rabbit jump modified, etc.
</commit_message>
<xml_diff>
--- a/할일정리파일.xlsx
+++ b/할일정리파일.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\Game_MoonRabbit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B15ACCF-5B41-4151-9487-E7D454DC8AC5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36D84869-30CB-49F3-8568-DA03147E1297}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1440" yWindow="300" windowWidth="11025" windowHeight="10320" xr2:uid="{A399527B-BAE3-45DA-870A-D71D4B42C21D}"/>
+    <workbookView xWindow="465" yWindow="165" windowWidth="11025" windowHeight="10320" xr2:uid="{A399527B-BAE3-45DA-870A-D71D4B42C21D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="64">
   <si>
     <t>프로그래밍</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -281,6 +281,28 @@
   </si>
   <si>
     <t>구슬 애니메이션이 destroy되기전에 먼저 이루어지도록 해야함.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>scrollview 위치 토끼위치로 변경</t>
+  </si>
+  <si>
+    <t>O</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>토끼 뛸 때 위치 anchoredposition 
+set</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>구슬 위치 조정(max_y:4, min_y:0.85)
+구슬 시작시 위에서 아래로</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>위치 조정 시 shooter.possible 불가능하게.
+애니메이션작동할때나 떨어질때 구슬과 부딪히는 현상 없게</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -657,10 +679,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AD2D038-EFC7-40D9-8F02-588A133B84E6}">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -755,7 +777,7 @@
         <v>38</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>40</v>
@@ -769,7 +791,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="C7" t="s">
         <v>23</v>
@@ -797,7 +819,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="C9" t="s">
         <v>28</v>
@@ -947,11 +969,17 @@
       <c r="A23" s="2" t="s">
         <v>48</v>
       </c>
+      <c r="B23" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="24" spans="1:4" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>50</v>
       </c>
+      <c r="B24" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
@@ -962,10 +990,48 @@
       <c r="A26" s="2" t="s">
         <v>57</v>
       </c>
+      <c r="B26" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="27" spans="1:4" ht="33" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>58</v>
+      </c>
+      <c r="B27" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>59</v>
+      </c>
+      <c r="B28" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="33" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B29" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B30" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="66" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B31" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
200215 ball modified, map add, resources add, item modified
</commit_message>
<xml_diff>
--- a/할일정리파일.xlsx
+++ b/할일정리파일.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\Game_MoonRabbit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36D84869-30CB-49F3-8568-DA03147E1297}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43FA105E-B8A4-46D3-A42C-930983302CC9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="465" yWindow="165" windowWidth="11025" windowHeight="10320" xr2:uid="{A399527B-BAE3-45DA-870A-D71D4B42C21D}"/>
+    <workbookView xWindow="810" yWindow="510" windowWidth="11025" windowHeight="10320" xr2:uid="{A399527B-BAE3-45DA-870A-D71D4B42C21D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="64">
   <si>
     <t>프로그래밍</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -217,10 +217,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>최준아</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>rowbomb, sixbomb 제일 밑에서 
 쏘면 폭탄 소리 안나고 구슬 쌓이는 소리 남</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -303,6 +299,13 @@
   <si>
     <t>위치 조정 시 shooter.possible 불가능하게.
 애니메이션작동할때나 떨어질때 구슬과 부딪히는 현상 없게</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>O
+Item1_Cnt,
+Item2_Cnt,
+Item3_Cnt</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -681,7 +684,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AD2D038-EFC7-40D9-8F02-588A133B84E6}">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -746,7 +749,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C4" t="s">
         <v>22</v>
@@ -844,16 +847,16 @@
     </row>
     <row r="11" spans="1:6" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" t="s">
         <v>51</v>
-      </c>
-      <c r="B11" t="s">
-        <v>52</v>
       </c>
       <c r="C11" t="s">
         <v>26</v>
       </c>
       <c r="D11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="33" x14ac:dyDescent="0.3">
@@ -872,7 +875,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="C13" t="s">
         <v>29</v>
@@ -913,7 +916,7 @@
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C17" t="s">
         <v>41</v>
@@ -930,7 +933,7 @@
         <v>34</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D18" t="s">
         <v>36</v>
@@ -951,87 +954,90 @@
     </row>
     <row r="21" spans="1:4" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" t="s">
         <v>44</v>
-      </c>
-      <c r="B21" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B24" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="66" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B26" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="33" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B27" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
+        <v>58</v>
+      </c>
+      <c r="B28" t="s">
         <v>59</v>
-      </c>
-      <c r="B28" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="33" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B29" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="66" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B31" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
200216 android check etc.
</commit_message>
<xml_diff>
--- a/할일정리파일.xlsx
+++ b/할일정리파일.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\Game_MoonRabbit\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Game_MoonRabbit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43FA105E-B8A4-46D3-A42C-930983302CC9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E42C4606-0CFF-4FAA-A9C6-D37F08399254}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="510" windowWidth="11025" windowHeight="10320" xr2:uid="{A399527B-BAE3-45DA-870A-D71D4B42C21D}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{A399527B-BAE3-45DA-870A-D71D4B42C21D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="64">
   <si>
     <t>프로그래밍</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -259,11 +259,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>송여령
-(쿠키런B)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>O</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -306,6 +301,10 @@
 Item1_Cnt,
 Item2_Cnt,
 Item3_Cnt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>O? 렉 많음</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -684,19 +683,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AD2D038-EFC7-40D9-8F02-588A133B84E6}">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="29.75" customWidth="1"/>
     <col min="2" max="2" width="10" customWidth="1"/>
     <col min="3" max="3" width="29.25" customWidth="1"/>
-    <col min="5" max="5" width="34.125" customWidth="1"/>
+    <col min="5" max="5" width="34.08203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -707,7 +706,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="66" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="68" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -727,12 +726,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C3" t="s">
         <v>21</v>
@@ -744,12 +743,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="33" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="C4" t="s">
         <v>22</v>
@@ -761,7 +760,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="33" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="34" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -775,7 +774,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="51" x14ac:dyDescent="0.45">
       <c r="A6" s="2" t="s">
         <v>38</v>
       </c>
@@ -789,7 +788,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="33" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="34" x14ac:dyDescent="0.45">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -803,7 +802,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="33" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="34" x14ac:dyDescent="0.45">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -817,7 +816,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="33" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="34" x14ac:dyDescent="0.45">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -831,7 +830,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -845,7 +844,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="51" x14ac:dyDescent="0.45">
       <c r="A11" s="2" t="s">
         <v>50</v>
       </c>
@@ -859,7 +858,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="33" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="34" x14ac:dyDescent="0.45">
       <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
@@ -870,7 +869,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
@@ -881,26 +880,29 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="C14" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="B15" t="s">
+        <v>63</v>
+      </c>
       <c r="C15" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
@@ -911,7 +913,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17" s="2" t="s">
         <v>17</v>
       </c>
@@ -925,7 +927,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="66" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" ht="51" x14ac:dyDescent="0.45">
       <c r="A18" s="2" t="s">
         <v>16</v>
       </c>
@@ -939,7 +941,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" ht="51" x14ac:dyDescent="0.45">
       <c r="A19" s="2" t="s">
         <v>35</v>
       </c>
@@ -947,12 +949,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A20" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" ht="51" x14ac:dyDescent="0.45">
       <c r="A21" s="2" t="s">
         <v>43</v>
       </c>
@@ -960,84 +962,84 @@
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A22" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B22" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A23" s="2" t="s">
         <v>47</v>
       </c>
       <c r="B23" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="49.5" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="51" x14ac:dyDescent="0.45">
       <c r="A24" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B24" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="68" x14ac:dyDescent="0.45">
+      <c r="A25" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="51" x14ac:dyDescent="0.45">
+      <c r="A26" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B26" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="34" x14ac:dyDescent="0.45">
+      <c r="A27" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B27" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A28" t="s">
+        <v>57</v>
+      </c>
+      <c r="B28" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="34" x14ac:dyDescent="0.45">
+      <c r="A29" s="2" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" ht="66" x14ac:dyDescent="0.3">
-      <c r="A25" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A26" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B26" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="33" x14ac:dyDescent="0.3">
-      <c r="A27" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B27" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+      <c r="B29" t="s">
         <v>58</v>
       </c>
-      <c r="B28" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="33" x14ac:dyDescent="0.3">
-      <c r="A29" s="2" t="s">
+    </row>
+    <row r="30" spans="1:4" ht="51" x14ac:dyDescent="0.45">
+      <c r="A30" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B29" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A30" s="2" t="s">
+      <c r="B30" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="68" x14ac:dyDescent="0.45">
+      <c r="A31" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B30" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="66" x14ac:dyDescent="0.3">
-      <c r="A31" s="2" t="s">
-        <v>62</v>
-      </c>
       <c r="B31" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
200222 item_text modified, limit_text modified, map modified, updown modified, etc.
</commit_message>
<xml_diff>
--- a/할일정리파일.xlsx
+++ b/할일정리파일.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Game_MoonRabbit\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\Game_MoonRabbit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B8519BB-F18A-4375-90F7-4C0A6E58D685}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A7F50EF-FC00-4FD3-804E-53E6F20E4830}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{A399527B-BAE3-45DA-870A-D71D4B42C21D}"/>
+    <workbookView xWindow="7500" yWindow="600" windowWidth="12930" windowHeight="10320" xr2:uid="{A399527B-BAE3-45DA-870A-D71D4B42C21D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="63">
   <si>
     <t>프로그래밍</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -297,6 +297,10 @@
 Item1_Cnt,
 Item2_Cnt,
 Item3_Cnt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>O</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -676,18 +680,18 @@
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="29.75" customWidth="1"/>
     <col min="2" max="2" width="10" customWidth="1"/>
     <col min="3" max="3" width="29.25" customWidth="1"/>
-    <col min="5" max="5" width="34.08203125" customWidth="1"/>
+    <col min="5" max="5" width="34.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -698,7 +702,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="68" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" ht="66" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -718,7 +722,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -735,7 +739,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -752,7 +756,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="34" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" ht="33" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -766,7 +770,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="51" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>38</v>
       </c>
@@ -780,7 +784,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="34" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" ht="33" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -794,7 +798,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="34" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" ht="33" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -808,7 +812,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="34" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" ht="33" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -822,7 +826,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -836,7 +840,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="51" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>49</v>
       </c>
@@ -850,10 +854,13 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="34" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" ht="33" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="B12" t="s">
+        <v>62</v>
+      </c>
       <c r="C12" t="s">
         <v>27</v>
       </c>
@@ -861,7 +868,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
@@ -872,7 +879,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
@@ -883,7 +890,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
@@ -894,7 +901,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
@@ -905,7 +912,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>17</v>
       </c>
@@ -919,7 +926,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="51" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:4" ht="66" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>16</v>
       </c>
@@ -933,7 +940,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="51" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:4" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>35</v>
       </c>
@@ -941,12 +948,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="51" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:4" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>43</v>
       </c>
@@ -954,7 +961,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>45</v>
       </c>
@@ -962,7 +969,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>46</v>
       </c>
@@ -970,7 +977,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="51" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:4" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>48</v>
       </c>
@@ -978,7 +985,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="68" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:4" ht="66" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>53</v>
       </c>
@@ -986,7 +993,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="51" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:4" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>54</v>
       </c>
@@ -994,7 +1001,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="34" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:4" ht="33" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>55</v>
       </c>
@@ -1002,7 +1009,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>56</v>
       </c>
@@ -1010,7 +1017,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="34" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:4" ht="33" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>58</v>
       </c>
@@ -1018,7 +1025,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="51" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:4" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>59</v>
       </c>
@@ -1026,7 +1033,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="68" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:4" ht="66" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>60</v>
       </c>

</xml_diff>